<commit_message>
XLSX para DOCX - Termo
</commit_message>
<xml_diff>
--- a/doc/modelo-excel.xlsx
+++ b/doc/modelo-excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\DocxNode\EditarWordEmMassa\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.almeida\Desktop\Vinicius\Desenvolvimento\EditarWordEmMassa\EditarWordEmMassa\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DD44F-2B30-4156-9BE4-0E78707A31F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F732BC3-609C-41A3-871C-DA683FDE2696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{39373C2D-9FBD-41AA-8512-C363176CBD90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{A29361A0-8B37-4701-BB33-982ED33EF05E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,55 +36,94 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>IDADE</t>
-  </si>
-  <si>
-    <t>CURSO</t>
-  </si>
-  <si>
-    <t>Vinicius</t>
-  </si>
-  <si>
-    <t>Ciência da Computação</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Fisioterapia</t>
-  </si>
-  <si>
-    <t>Antônio</t>
-  </si>
-  <si>
-    <t>Engenharia de Software</t>
-  </si>
-  <si>
-    <t>Raphael</t>
-  </si>
-  <si>
-    <t>Análise e Desenvolvimento de Sistemas</t>
-  </si>
-  <si>
-    <t>Vidal</t>
-  </si>
-  <si>
-    <t>Duda</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>COLABORADOR</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>MODELO</t>
+  </si>
+  <si>
+    <t>NOTEBOOK</t>
+  </si>
+  <si>
+    <t>SERIAL</t>
+  </si>
+  <si>
+    <t>PATRIMONIO</t>
+  </si>
+  <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>000.000.000-00</t>
+  </si>
+  <si>
+    <t>MARCA 001 A1</t>
+  </si>
+  <si>
+    <t>MARCA 002 G2</t>
+  </si>
+  <si>
+    <t>NOTEBOOK 1</t>
+  </si>
+  <si>
+    <t>NOTEBOOK 2</t>
+  </si>
+  <si>
+    <t>S0001</t>
+  </si>
+  <si>
+    <t>S0002</t>
+  </si>
+  <si>
+    <t>SÃO PAULO</t>
+  </si>
+  <si>
+    <t>BELO HORIZONTE</t>
+  </si>
+  <si>
+    <t>JANEIRO</t>
+  </si>
+  <si>
+    <t>FEVEREIRO</t>
+  </si>
+  <si>
+    <t>FULANO DA SILVA</t>
+  </si>
+  <si>
+    <t>CICLANO SOUZA</t>
+  </si>
+  <si>
+    <t>999.999.999-99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,8 +149,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,93 +496,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C13C5C-8778-4C38-93E4-49B7033451AF}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E46802-8734-4AC6-B648-5444313B4FBE}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1001</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="J2" s="1">
+        <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1002</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>